<commit_message>
update em plano de projetos, documentação de requisitos e na planilha de ICs
</commit_message>
<xml_diff>
--- a/documentação/planilha/planilha de ICs - Next Page.xlsx
+++ b/documentação/planilha/planilha de ICs - Next Page.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -43,6 +43,9 @@
     <t xml:space="preserve">Relacionamentos</t>
   </si>
   <si>
+    <t xml:space="preserve">Baseline </t>
+  </si>
+  <si>
     <t xml:space="preserve">IC-001</t>
   </si>
   <si>
@@ -52,7 +55,7 @@
     <t xml:space="preserve">Documentação de planejamento</t>
   </si>
   <si>
-    <t xml:space="preserve">C-001</t>
+    <t xml:space="preserve">0.1</t>
   </si>
   <si>
     <t xml:space="preserve">Gerente</t>
@@ -73,7 +76,7 @@
     <t xml:space="preserve">Especificação de requisitos</t>
   </si>
   <si>
-    <t xml:space="preserve">C-002</t>
+    <t xml:space="preserve">0.2</t>
   </si>
   <si>
     <t xml:space="preserve">PO</t>
@@ -118,6 +121,9 @@
     <t xml:space="preserve">Lista de requisitos</t>
   </si>
   <si>
+    <t xml:space="preserve">0.3</t>
+  </si>
+  <si>
     <t xml:space="preserve">PO/analista</t>
   </si>
   <si>
@@ -160,7 +166,7 @@
     <t xml:space="preserve">Dev</t>
   </si>
   <si>
-    <t xml:space="preserve">IC-003,IC-004</t>
+    <t xml:space="preserve">IC-003,IC-004,IC-006,IC-007</t>
   </si>
   <si>
     <t xml:space="preserve">IC-009</t>
@@ -226,14 +232,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -246,6 +244,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -310,8 +314,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -513,19 +517,20 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="40.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="43.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="29.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="54.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="31.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -550,255 +555,287 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3"/>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>13</v>
+      <c r="F2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="C3" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="D3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="F3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="D4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="F4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="C5" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="D5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>28</v>
+        <v>11</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="C6" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="D6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="5" t="s">
         <v>33</v>
       </c>
+      <c r="E6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="B7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="D7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>37</v>
+      <c r="H10" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="B11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>37</v>
+        <v>11</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>